<commit_message>
making the read function more flexible
</commit_message>
<xml_diff>
--- a/dataframe.xlsx
+++ b/dataframe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>img</t>
+          <t>imgFileName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -461,13 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[227 248 277 ... 238 275 272]
- [215 236 264 ... 255 299 309]
- [214 221 248 ... 287 342 351]
- ...
- [151 151 161 ... 344 358 362]
- [158 161 172 ... 338 351 352]
- [158 161 171 ... 340 346 343]]</t>
+          <t>convertedZVIImage1.png</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -477,106 +471,6 @@
         <v>0.511904761904762</v>
       </c>
       <c r="E2" t="n">
-        <v>0.511904761904762</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>[[227 248 277 ... 238 275 272]
- [215 236 264 ... 255 299 309]
- [214 221 248 ... 287 342 351]
- ...
- [151 151 161 ... 344 358 362]
- [158 161 172 ... 338 351 352]
- [158 161 171 ... 340 346 343]]</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.064</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.511904761904762</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.511904761904762</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>[[227 248 277 ... 238 275 272]
- [215 236 264 ... 255 299 309]
- [214 221 248 ... 287 342 351]
- ...
- [151 151 161 ... 344 358 362]
- [158 161 172 ... 338 351 352]
- [158 161 171 ... 340 346 343]]</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.064</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.511904761904762</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.511904761904762</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>[[227 248 277 ... 238 275 272]
- [215 236 264 ... 255 299 309]
- [214 221 248 ... 287 342 351]
- ...
- [151 151 161 ... 344 358 362]
- [158 161 172 ... 338 351 352]
- [158 161 171 ... 340 346 343]]</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.064</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.511904761904762</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.511904761904762</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>[[227 248 277 ... 238 275 272]
- [215 236 264 ... 255 299 309]
- [214 221 248 ... 287 342 351]
- ...
- [151 151 161 ... 344 358 362]
- [158 161 172 ... 338 351 352]
- [158 161 171 ... 340 346 343]]</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.064</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.511904761904762</v>
-      </c>
-      <c r="E6" t="n">
         <v>0.511904761904762</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finishig the revision on the readConvertZVIFile function
</commit_message>
<xml_diff>
--- a/dataframe.xlsx
+++ b/dataframe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>convertedZVIImage1.png</t>
+          <t>sampleFile2.zvi_filtered1.png</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -471,6 +471,82 @@
         <v>0.511904761904762</v>
       </c>
       <c r="E2" t="n">
+        <v>0.511904761904762</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sampleFile3.zvi_filtered2.png</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.511904761904762</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.511904761904762</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sampleFile4.zvi_filtered3.png</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.511904761904762</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.511904761904762</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sampleFile1.zvi_filtered4.png</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.511904761904762</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.511904761904762</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sampleFile5.zvi_filtered5.png</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.511904761904762</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.511904761904762</v>
       </c>
     </row>

</xml_diff>